<commit_message>
Corrections based on first round debugging
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
+++ b/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_Artelys/add-outputs/BDbDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{CB5A19F7-E7B7-429A-B0D9-60CDB12B96F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BEB29A0-01DB-4A98-9E9A-D19348ADFEDB}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{CB5A19F7-E7B7-429A-B0D9-60CDB12B96F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{589B4295-4CA9-4DD1-BE9B-58D3CB34CD71}"/>
   <bookViews>
-    <workbookView xWindow="9570" yWindow="0" windowWidth="9720" windowHeight="11370" xr2:uid="{A7EE9673-2FA7-4CC3-AB75-B5BA10698243}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{A7EE9673-2FA7-4CC3-AB75-B5BA10698243}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>BDbDT BAU Deaths by Demographic Traits</t>
   </si>
@@ -131,6 +131,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>asian</t>
+  </si>
+  <si>
+    <t>other race</t>
+  </si>
+  <si>
+    <t>hispanic</t>
+  </si>
+  <si>
+    <t>nonhispanic</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22DD064-0018-4998-8480-8846E6E1D8EE}">
   <dimension ref="B11:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3565,127 +3583,127 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <f>B2/2</f>
+        <f t="shared" ref="B3:AF3" si="1">B2/2</f>
         <v>2592038.5</v>
       </c>
       <c r="C3">
-        <f>C2/2</f>
+        <f t="shared" si="1"/>
         <v>2650000</v>
       </c>
       <c r="D3">
-        <f>D2/2</f>
+        <f t="shared" si="1"/>
         <v>2574297.5</v>
       </c>
       <c r="E3">
-        <f>E2/2</f>
+        <f t="shared" si="1"/>
         <v>2511877.5</v>
       </c>
       <c r="F3">
-        <f>F2/2</f>
+        <f t="shared" si="1"/>
         <v>2494421</v>
       </c>
       <c r="G3">
-        <f>G2/2</f>
+        <f t="shared" si="1"/>
         <v>2502488</v>
       </c>
       <c r="H3">
-        <f>H2/2</f>
+        <f t="shared" si="1"/>
         <v>2510021.5</v>
       </c>
       <c r="I3">
-        <f>I2/2</f>
+        <f t="shared" si="1"/>
         <v>2517184.5</v>
       </c>
       <c r="J3">
-        <f>J2/2</f>
+        <f t="shared" si="1"/>
         <v>2524294.5</v>
       </c>
       <c r="K3">
-        <f>K2/2</f>
+        <f t="shared" si="1"/>
         <v>2531614</v>
       </c>
       <c r="L3">
-        <f>L2/2</f>
+        <f t="shared" si="1"/>
         <v>2539393.5</v>
       </c>
       <c r="M3">
-        <f>M2/2</f>
+        <f t="shared" si="1"/>
         <v>2547771.5</v>
       </c>
       <c r="N3">
-        <f>N2/2</f>
+        <f t="shared" si="1"/>
         <v>2557049.5</v>
       </c>
       <c r="O3">
-        <f>O2/2</f>
+        <f t="shared" si="1"/>
         <v>2567338.5</v>
       </c>
       <c r="P3">
-        <f>P2/2</f>
+        <f t="shared" si="1"/>
         <v>2579123.5</v>
       </c>
       <c r="Q3">
-        <f>Q2/2</f>
+        <f t="shared" si="1"/>
         <v>2592343.5</v>
       </c>
       <c r="R3">
-        <f>R2/2</f>
+        <f t="shared" si="1"/>
         <v>2606614</v>
       </c>
       <c r="S3">
-        <f>S2/2</f>
+        <f t="shared" si="1"/>
         <v>2621809.5</v>
       </c>
       <c r="T3">
-        <f>T2/2</f>
+        <f t="shared" si="1"/>
         <v>2637784</v>
       </c>
       <c r="U3">
-        <f>U2/2</f>
+        <f t="shared" si="1"/>
         <v>2654278</v>
       </c>
       <c r="V3">
-        <f>V2/2</f>
+        <f t="shared" si="1"/>
         <v>2671030.5</v>
       </c>
       <c r="W3">
-        <f>W2/2</f>
+        <f t="shared" si="1"/>
         <v>2687685.5</v>
       </c>
       <c r="X3">
-        <f>X2/2</f>
+        <f t="shared" si="1"/>
         <v>2704236</v>
       </c>
       <c r="Y3">
-        <f>Y2/2</f>
+        <f t="shared" si="1"/>
         <v>2720443.5</v>
       </c>
       <c r="Z3">
-        <f>Z2/2</f>
+        <f t="shared" si="1"/>
         <v>2736060.5</v>
       </c>
       <c r="AA3">
-        <f>AA2/2</f>
+        <f t="shared" si="1"/>
         <v>2750919</v>
       </c>
       <c r="AB3">
-        <f>AB2/2</f>
+        <f t="shared" si="1"/>
         <v>2765266</v>
       </c>
       <c r="AC3">
-        <f>AC2/2</f>
+        <f t="shared" si="1"/>
         <v>2778586.5</v>
       </c>
       <c r="AD3">
-        <f>AD2/2</f>
+        <f t="shared" si="1"/>
         <v>2791009</v>
       </c>
       <c r="AE3">
-        <f>AE2/2</f>
+        <f t="shared" si="1"/>
         <v>2802604</v>
       </c>
       <c r="AF3">
-        <f>AF2/2</f>
+        <f t="shared" si="1"/>
         <v>2813424.5</v>
       </c>
     </row>
@@ -3694,127 +3712,127 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f>B2/2</f>
+        <f t="shared" ref="B4:AF4" si="2">B2/2</f>
         <v>2592038.5</v>
       </c>
       <c r="C4">
-        <f>C2/2</f>
+        <f t="shared" si="2"/>
         <v>2650000</v>
       </c>
       <c r="D4">
-        <f>D2/2</f>
+        <f t="shared" si="2"/>
         <v>2574297.5</v>
       </c>
       <c r="E4">
-        <f>E2/2</f>
+        <f t="shared" si="2"/>
         <v>2511877.5</v>
       </c>
       <c r="F4">
-        <f>F2/2</f>
+        <f t="shared" si="2"/>
         <v>2494421</v>
       </c>
       <c r="G4">
-        <f>G2/2</f>
+        <f t="shared" si="2"/>
         <v>2502488</v>
       </c>
       <c r="H4">
-        <f>H2/2</f>
+        <f t="shared" si="2"/>
         <v>2510021.5</v>
       </c>
       <c r="I4">
-        <f>I2/2</f>
+        <f t="shared" si="2"/>
         <v>2517184.5</v>
       </c>
       <c r="J4">
-        <f>J2/2</f>
+        <f t="shared" si="2"/>
         <v>2524294.5</v>
       </c>
       <c r="K4">
-        <f>K2/2</f>
+        <f t="shared" si="2"/>
         <v>2531614</v>
       </c>
       <c r="L4">
-        <f>L2/2</f>
+        <f t="shared" si="2"/>
         <v>2539393.5</v>
       </c>
       <c r="M4">
-        <f>M2/2</f>
+        <f t="shared" si="2"/>
         <v>2547771.5</v>
       </c>
       <c r="N4">
-        <f>N2/2</f>
+        <f t="shared" si="2"/>
         <v>2557049.5</v>
       </c>
       <c r="O4">
-        <f>O2/2</f>
+        <f t="shared" si="2"/>
         <v>2567338.5</v>
       </c>
       <c r="P4">
-        <f>P2/2</f>
+        <f t="shared" si="2"/>
         <v>2579123.5</v>
       </c>
       <c r="Q4">
-        <f>Q2/2</f>
+        <f t="shared" si="2"/>
         <v>2592343.5</v>
       </c>
       <c r="R4">
-        <f>R2/2</f>
+        <f t="shared" si="2"/>
         <v>2606614</v>
       </c>
       <c r="S4">
-        <f>S2/2</f>
+        <f t="shared" si="2"/>
         <v>2621809.5</v>
       </c>
       <c r="T4">
-        <f>T2/2</f>
+        <f t="shared" si="2"/>
         <v>2637784</v>
       </c>
       <c r="U4">
-        <f>U2/2</f>
+        <f t="shared" si="2"/>
         <v>2654278</v>
       </c>
       <c r="V4">
-        <f>V2/2</f>
+        <f t="shared" si="2"/>
         <v>2671030.5</v>
       </c>
       <c r="W4">
-        <f>W2/2</f>
+        <f t="shared" si="2"/>
         <v>2687685.5</v>
       </c>
       <c r="X4">
-        <f>X2/2</f>
+        <f t="shared" si="2"/>
         <v>2704236</v>
       </c>
       <c r="Y4">
-        <f>Y2/2</f>
+        <f t="shared" si="2"/>
         <v>2720443.5</v>
       </c>
       <c r="Z4">
-        <f>Z2/2</f>
+        <f t="shared" si="2"/>
         <v>2736060.5</v>
       </c>
       <c r="AA4">
-        <f>AA2/2</f>
+        <f t="shared" si="2"/>
         <v>2750919</v>
       </c>
       <c r="AB4">
-        <f>AB2/2</f>
+        <f t="shared" si="2"/>
         <v>2765266</v>
       </c>
       <c r="AC4">
-        <f>AC2/2</f>
+        <f t="shared" si="2"/>
         <v>2778586.5</v>
       </c>
       <c r="AD4">
-        <f>AD2/2</f>
+        <f t="shared" si="2"/>
         <v>2791009</v>
       </c>
       <c r="AE4">
-        <f>AE2/2</f>
+        <f t="shared" si="2"/>
         <v>2802604</v>
       </c>
       <c r="AF4">
-        <f>AF2/2</f>
+        <f t="shared" si="2"/>
         <v>2813424.5</v>
       </c>
     </row>
@@ -3828,10 +3846,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4222,32 +4240,600 @@
         <v>2813424.5</v>
       </c>
     </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -4470,10 +5056,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAC407-2C23-460B-9EB1-6E0FD9611CFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEE1E253-46C7-4725-AA2F-676C05BF78A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4490,20 +5107,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEE1E253-46C7-4725-AA2F-676C05BF78A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAC407-2C23-460B-9EB1-6E0FD9611CFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data file correction, csv export
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
+++ b/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_Artelys/add-outputs/BDbDT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\add-outputs\BDbDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{CB5A19F7-E7B7-429A-B0D9-60CDB12B96F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{589B4295-4CA9-4DD1-BE9B-58D3CB34CD71}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16ADA03-60D3-4D16-9047-8AF2519A04AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{A7EE9673-2FA7-4CC3-AB75-B5BA10698243}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>BDbDT BAU Deaths by Demographic Traits</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>nonhispanic</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -3848,16 +3854,14 @@
   </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:AF9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="A1" s="21"/>
       <c r="B1">
         <v>2020</v>
       </c>
@@ -3984,7 +3988,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <f>Calcs!B3</f>
@@ -4113,7 +4117,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <f>Calcs!B4</f>
@@ -4834,6 +4838,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -5056,27 +5080,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAC407-2C23-460B-9EB1-6E0FD9611CFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71105CF5-44B5-4E3D-ABCC-9AA2F9B21790}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEE1E253-46C7-4725-AA2F-676C05BF78A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5093,23 +5116,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71105CF5-44B5-4E3D-ABCC-9AA2F9B21790}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAC407-2C23-460B-9EB1-6E0FD9611CFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>